<commit_message>
working infra_year_timeslices, need to be improved
</commit_message>
<xml_diff>
--- a/default/4 - infra_year_timeslices/model/input_data/input_data.xlsx
+++ b/default/4 - infra_year_timeslices/model/input_data/input_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baioc\Documents\GitHub\pyesm\default\prove_vale\model\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baioc\Documents\GitHub\pyesm\default\4 - infra_year_timeslices\model\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9699FFEE-C88A-4B43-9092-2573143915A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3017F3-8333-45E2-942F-C0752EC81065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="u" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,12 @@
     <sheet name="lf_min" sheetId="6" r:id="rId6"/>
     <sheet name="cap_year_y" sheetId="7" r:id="rId7"/>
     <sheet name="dp" sheetId="8" r:id="rId8"/>
-    <sheet name="n_periods" sheetId="10" r:id="rId9"/>
+    <sheet name="n_periods" sheetId="9" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">d!$E$1:$E$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">u!$E$1:$E$13</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -55,6 +59,9 @@
     <t>flows_agg_Names</t>
   </si>
   <si>
+    <t>years</t>
+  </si>
+  <si>
     <t>values</t>
   </si>
   <si>
@@ -65,6 +72,12 @@
   </si>
   <si>
     <t>EE</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y2</t>
   </si>
   <si>
     <t>Coal</t>
@@ -83,15 +96,6 @@
   </si>
   <si>
     <t>EE_Coal</t>
-  </si>
-  <si>
-    <t>years</t>
-  </si>
-  <si>
-    <t>y1</t>
-  </si>
-  <si>
-    <t>y2</t>
   </si>
   <si>
     <t>hours</t>
@@ -122,6 +126,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -467,15 +472,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F8" sqref="F8:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,125 +496,271 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E5">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E7">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:E13" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F13">
+      <sortCondition ref="E1:E13"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,166 +771,381 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>8</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:E19" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F19">
+      <sortCondition ref="E1:E19"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -789,7 +1155,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +1171,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -813,10 +1179,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>0.5</v>
@@ -827,10 +1193,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -841,10 +1207,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>0.01</v>
@@ -860,7 +1226,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,10 +1242,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -887,13 +1253,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>1000</v>
@@ -904,13 +1270,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>1500</v>
@@ -921,13 +1287,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -938,13 +1304,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>50</v>
@@ -960,13 +1326,10 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F2" sqref="F2:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -982,10 +1345,10 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -993,16 +1356,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1013,16 +1376,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1033,16 +1396,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>0.3</v>
@@ -1053,16 +1416,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>0.3</v>
@@ -1073,16 +1436,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>0.2</v>
@@ -1093,16 +1456,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>0.2</v>
@@ -1113,16 +1476,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <v>0.9</v>
@@ -1133,16 +1496,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F9">
         <v>0.9</v>
@@ -1153,16 +1516,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <v>0.9</v>
@@ -1173,16 +1536,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F11">
         <v>0.9</v>
@@ -1193,16 +1556,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>0.9</v>
@@ -1213,16 +1576,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F13">
         <v>0.9</v>
@@ -1233,16 +1596,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1253,16 +1616,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1273,16 +1636,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1293,16 +1656,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1313,16 +1676,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1333,16 +1696,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1358,7 +1721,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F19"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,10 +1740,10 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1388,16 +1751,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1408,16 +1771,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1428,16 +1791,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1448,16 +1811,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1468,16 +1831,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1488,16 +1851,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1508,16 +1871,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1528,16 +1891,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1548,16 +1911,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1568,16 +1931,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1588,16 +1951,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1608,16 +1971,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1628,16 +1991,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1648,16 +2011,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1668,16 +2031,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1688,16 +2051,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1708,16 +2071,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1728,16 +2091,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1753,7 +2116,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,10 +2132,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1780,13 +2143,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>5000</v>
@@ -1797,13 +2160,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>8000</v>
@@ -1814,13 +2177,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>2500</v>
@@ -1831,13 +2194,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>5000</v>
@@ -1848,13 +2211,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <v>2500</v>
@@ -1865,13 +2228,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>2500</v>
@@ -1887,7 +2250,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E7"/>
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +2269,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1914,10 +2277,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -1931,10 +2294,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -1948,10 +2311,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -1965,10 +2328,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -1983,10 +2346,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -2001,10 +2364,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -2020,11 +2383,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2037,7 +2400,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2045,7 +2408,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>365</v>

</xml_diff>